<commit_message>
Fixed issue where rank of all higher taxa was assigned as "genus" in Materials sheet, as well as generalising "casting out genera" algorithm - three higher taxa are left in excess
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Chaetognatha.xlsx
+++ b/data/dataPaper-I-in/arphified/Chaetognatha.xlsx
@@ -1896,7 +1896,7 @@
         <v>36</v>
       </c>
       <c r="AF2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AG2" t="s">
         <v>36</v>
@@ -1932,7 +1932,7 @@
         <v>36</v>
       </c>
       <c r="AR2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AS2" t="s">
         <v>36</v>
@@ -1941,7 +1941,7 @@
         <v>36</v>
       </c>
       <c r="AU2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AV2" t="s">
         <v>36</v>
@@ -2363,7 +2363,7 @@
         <v>36</v>
       </c>
       <c r="AF3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AG3" t="s">
         <v>36</v>
@@ -2399,7 +2399,7 @@
         <v>36</v>
       </c>
       <c r="AR3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AS3" t="s">
         <v>36</v>
@@ -2408,7 +2408,7 @@
         <v>36</v>
       </c>
       <c r="AU3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AV3" t="s">
         <v>36</v>
@@ -2830,7 +2830,7 @@
         <v>36</v>
       </c>
       <c r="AF4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AG4" t="s">
         <v>36</v>
@@ -2866,7 +2866,7 @@
         <v>36</v>
       </c>
       <c r="AR4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AS4" t="s">
         <v>36</v>
@@ -2875,7 +2875,7 @@
         <v>36</v>
       </c>
       <c r="AU4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AV4" t="s">
         <v>36</v>
@@ -3297,7 +3297,7 @@
         <v>36</v>
       </c>
       <c r="AF5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AG5" t="s">
         <v>36</v>
@@ -3333,7 +3333,7 @@
         <v>36</v>
       </c>
       <c r="AR5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AS5" t="s">
         <v>36</v>
@@ -3342,7 +3342,7 @@
         <v>36</v>
       </c>
       <c r="AU5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AV5" t="s">
         <v>36</v>
@@ -3764,7 +3764,7 @@
         <v>36</v>
       </c>
       <c r="AF6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AG6" t="s">
         <v>36</v>
@@ -3800,7 +3800,7 @@
         <v>36</v>
       </c>
       <c r="AR6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AS6" t="s">
         <v>36</v>
@@ -3809,7 +3809,7 @@
         <v>36</v>
       </c>
       <c r="AU6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AV6" t="s">
         <v>36</v>

</xml_diff>